<commit_message>
10/04/2023 updated excel of Demands.xlsx
</commit_message>
<xml_diff>
--- a/docs/Demands.xlsx
+++ b/docs/Demands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\Documents\GitHub\ADSS_Group_H\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasmo\Documents\ADSS_Group_H\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354967A7-F2D5-45B4-A2D9-465F1BC89DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660CB926-0265-44EA-BAB8-26742F1FF245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{329DF1D6-0C91-4AE4-AB6F-B4D8B4970C8F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{329DF1D6-0C91-4AE4-AB6F-B4D8B4970C8F}"/>
   </bookViews>
   <sheets>
     <sheet name="דרישות" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="111">
   <si>
     <t>ID</t>
   </si>
@@ -64,15 +64,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>Suppliers</t>
-  </si>
-  <si>
-    <t>responsibility</t>
-  </si>
-  <si>
-    <t>The system must have a weight of each potential product that the warehouse might order</t>
-  </si>
-  <si>
     <t>Functional\None Functional</t>
   </si>
   <si>
@@ -109,9 +100,6 @@
     <t>The system can show truck's details such as truck max weight, weight, drivers license needed to drive</t>
   </si>
   <si>
-    <t xml:space="preserve">When adding a new driver, the system must inforce inserting a driving license type </t>
-  </si>
-  <si>
     <t>Isuue</t>
   </si>
   <si>
@@ -148,28 +136,10 @@
     <t>what type of trucks are available?</t>
   </si>
   <si>
-    <t>trucks that are more than 3.5 ton and less than 12 ton, and trucks that are more than 12 tons.</t>
-  </si>
-  <si>
     <t>what type of drivers license are available?</t>
   </si>
   <si>
-    <t>there are 2 drivers license: C,C1. C can drive all trucks, C1 can only drive the smaller trucks.</t>
-  </si>
-  <si>
     <t>how does the system engage a failure in a delivery?</t>
-  </si>
-  <si>
-    <t>the system will show an error if a failure acure due to a maxweight violation, and the user must create a new delivery.</t>
-  </si>
-  <si>
-    <t>storage</t>
-  </si>
-  <si>
-    <t>each product in the system must have a weight.</t>
-  </si>
-  <si>
-    <t>each order that the delivery system receive, must contain each product with its amounts, and its weight. And a total weight of the order.</t>
   </si>
   <si>
     <t>should the system prepare to an overweight incident?</t>
@@ -383,21 +353,42 @@
   <si>
     <t xml:space="preserve">הסר הזמנה ???? </t>
   </si>
+  <si>
+    <t>there are 2 drivers license: C,C1. C can drive all trucks, C1 can only drive the smaller trucks. Also, there is a qualification to drive a cooler truck that only specific drivers can know</t>
+  </si>
+  <si>
+    <t>trucks that are more than 3.5 ton and less than 12 ton, and trucks that are more than 12 tons.Also, there is truck with special qualifications, such as coolertrucks</t>
+  </si>
+  <si>
+    <t>the system will show an error if a failure acure due to a maxweight violation, and will show him the options to resolve it</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>The system must support adding Orders in a way that the user has to add how much of each product he wants</t>
+  </si>
+  <si>
+    <t>which transit can be executed?</t>
+  </si>
+  <si>
+    <t>only orders that the due date is the same date as today can be executed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="David"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="David"/>
       <family val="2"/>
     </font>
@@ -435,49 +426,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -536,55 +490,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="13">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -596,21 +535,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="David"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -764,16 +688,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20622493-A0C2-4802-86E8-E251779236A7}" name="Table1" displayName="Table1" ref="A1:H28" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{76ACBACD-D979-46ED-AD24-263B6B1A451C}" name="ID" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{DE128EAB-530B-4211-A440-48F608E85F90}" name="Module" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{0AB79CEE-5753-448F-8662-A6A9FF455379}" name="Functional\None Functional" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{D2EF77BC-C8DD-4D9A-A33B-89B6EF391906}" name="Description" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{31A5687C-5203-44A4-9037-FBF1CA81E1BA}" name="Priority" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{6ECB6A27-EBE8-400C-B948-2DA37B95E9B3}" name="Risk" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{A4F2648F-8594-4EBD-8F8D-EBA370698242}" name="Status" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{4EFB6FBD-1550-4814-8A4D-365FE2AB8B16}" name="responsibility" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20622493-A0C2-4802-86E8-E251779236A7}" name="Table1" displayName="Table1" ref="A1:G19" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{76ACBACD-D979-46ED-AD24-263B6B1A451C}" name="ID" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{DE128EAB-530B-4211-A440-48F608E85F90}" name="Module" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{0AB79CEE-5753-448F-8662-A6A9FF455379}" name="Functional\None Functional" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{D2EF77BC-C8DD-4D9A-A33B-89B6EF391906}" name="Description" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{31A5687C-5203-44A4-9037-FBF1CA81E1BA}" name="Priority" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{6ECB6A27-EBE8-400C-B948-2DA37B95E9B3}" name="Risk" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{A4F2648F-8594-4EBD-8F8D-EBA370698242}" name="Status" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1071,23 +994,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1530C2-D1E7-4CA0-8167-19AAD01E139D}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="25.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.25" customWidth="1"/>
-    <col min="5" max="5" width="9.75" customWidth="1"/>
+    <col min="3" max="3" width="25.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.19921875" customWidth="1"/>
+    <col min="5" max="5" width="9.69921875" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1095,7 +1017,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1109,11 +1031,8 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="55.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1121,23 +1040,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="82.8" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="84" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1145,23 +1063,22 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1169,25 +1086,22 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1195,25 +1109,22 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1221,43 +1132,45 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>63</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1265,23 +1178,22 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="84" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1289,23 +1201,22 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="55.2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1313,23 +1224,22 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="82.8" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="126" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1337,23 +1247,22 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="98" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1361,23 +1270,22 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="124.2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1385,23 +1293,22 @@
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" ht="96.6" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1409,23 +1316,22 @@
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" ht="69" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1433,23 +1339,22 @@
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="55.2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="56" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1457,47 +1362,35 @@
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" ht="55.2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1509,9 +1402,8 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1523,160 +1415,6 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>30</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="6"/>
-    </row>
-    <row r="30" spans="1:8" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>31</v>
-      </c>
-      <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>42</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1692,99 +1430,99 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="1" max="1" width="11.59765625" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="30.375" customWidth="1"/>
-    <col min="4" max="4" width="11.625" customWidth="1"/>
+    <col min="3" max="3" width="30.3984375" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1805,77 +1543,77 @@
       <selection activeCell="C7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E3" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" t="s">
-        <v>56</v>
-      </c>
       <c r="G3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
         <v>49</v>
       </c>
-      <c r="E5" t="s">
-        <v>59</v>
-      </c>
       <c r="F5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1887,127 +1625,131 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748931EE-FFC9-4ACF-A94C-2B9106A4C9E1}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.125" customWidth="1"/>
+    <col min="2" max="2" width="33.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="56" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2025,96 +1767,96 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.875" customWidth="1"/>
-    <col min="12" max="12" width="11.25" customWidth="1"/>
-    <col min="13" max="13" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.8984375" customWidth="1"/>
+    <col min="12" max="12" width="11.19921875" customWidth="1"/>
+    <col min="13" max="13" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>83</v>
+      <c r="C1" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="M1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>5</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6</v>
       </c>
@@ -2128,234 +1870,234 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761DE016-E18B-4A3A-8C5B-7EB06D18C272}">
   <dimension ref="B1:D32"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView rightToLeft="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.09765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="10"/>
+      <c r="C2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="10"/>
+      <c r="C3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="10"/>
+      <c r="C6" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="10"/>
+      <c r="C7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="10"/>
+      <c r="C10" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="10"/>
+      <c r="C11" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="10"/>
+      <c r="C12" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="10"/>
+      <c r="C13" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="12" t="s">
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="12"/>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
-      <c r="C3" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="12"/>
+      <c r="C18" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="12"/>
+      <c r="C19" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="12"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="14"/>
-      <c r="C6" s="12" t="s">
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="12"/>
+      <c r="C20" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="12" t="s">
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="12"/>
+      <c r="C21" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
-      <c r="C10" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="14"/>
-      <c r="C13" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" s="12"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="16"/>
-      <c r="C18" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="16"/>
-      <c r="C19" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="16"/>
-      <c r="C20" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="16"/>
-      <c r="C21" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="12"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="17"/>
-      <c r="C22" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="13"/>
+      <c r="C22" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>